<commit_message>
Update r code and files
</commit_message>
<xml_diff>
--- a/output/output_parametric_survival_model_parameters.xlsx
+++ b/output/output_parametric_survival_model_parameters.xlsx
@@ -1,52 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/ahem_r_assignments/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33186EEE-5D74-0943-AC95-B49037FC63A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="740" yWindow="660" windowWidth="13120" windowHeight="7040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PFS caba" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PFS mito" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="OS caba" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="OS mito" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PFS caba" sheetId="1" r:id="rId1"/>
+    <sheet name="PFS mito" sheetId="2" r:id="rId2"/>
+    <sheet name="OS caba" sheetId="3" r:id="rId3"/>
+    <sheet name="OS mito" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
-    <t xml:space="preserve"/>
+    <t/>
   </si>
   <si>
-    <t xml:space="preserve">exponential</t>
+    <t>exponential</t>
   </si>
   <si>
-    <t xml:space="preserve">weibull</t>
+    <t>weibull</t>
   </si>
   <si>
-    <t xml:space="preserve">lognormal</t>
+    <t>lognormal</t>
   </si>
   <si>
-    <t xml:space="preserve">loglogistic</t>
+    <t>loglogistic</t>
   </si>
   <si>
-    <t xml:space="preserve">AIC</t>
+    <t>AIC</t>
   </si>
   <si>
-    <t xml:space="preserve">intercept</t>
+    <t>intercept</t>
   </si>
   <si>
-    <t xml:space="preserve">log(scale)</t>
+    <t>log(scale)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -82,6 +102,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -363,17 +392,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF7F50"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="B2:C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,73 +421,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1885.1071</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1885.1070999999999</v>
+      </c>
+      <c r="C2">
         <v>1885.5943</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1886.6016</v>
       </c>
-      <c r="E2" t="n">
-        <v>1895.3382</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="E2">
+        <v>1895.3381999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.4561</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.4383</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.9282</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.9382</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>1.4560999999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.4382999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.92820000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0.93820000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>0.0566</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="D4">
         <v>0.1527</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.3479</v>
+      <c r="E4">
+        <v>-0.34789999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFCD5B45"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,73 +505,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1754.2742</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1754.2742000000001</v>
+      </c>
+      <c r="C2">
         <v>1748.7375</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1691.7935</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1695.7627</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1.1368</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1.0851</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.584</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E3">
         <v>0.5222</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.1132</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.0635</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="E4">
         <v>-0.4662</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF87CEEB"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,73 +589,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1987.5033</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1939.5375</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B2">
+        <v>1987.5033000000001</v>
+      </c>
+      <c r="C2">
+        <v>1939.5374999999999</v>
+      </c>
+      <c r="D2">
         <v>1952.9809</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1938.9274</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>3.0551</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3.0125</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.705</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.723</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>3.0550999999999999</v>
+      </c>
+      <c r="C3">
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="D3">
+        <v>2.7050000000000001</v>
+      </c>
+      <c r="E3">
+        <v>2.7229999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>-0.405</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>-0.40500000000000003</v>
+      </c>
+      <c r="D4">
         <v>-0.1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>-0.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF4A708B"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,57 +673,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>2019.9897</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1948.8256</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1966.3671</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="B2">
+        <v>2019.9897000000001</v>
+      </c>
+      <c r="C2">
+        <v>1948.8255999999999</v>
+      </c>
+      <c r="D2">
+        <v>1966.3670999999999</v>
+      </c>
+      <c r="E2">
         <v>1948.9386</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>2.7684</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3">
+        <v>2.7684000000000002</v>
+      </c>
+      <c r="C3">
         <v>2.778</v>
       </c>
-      <c r="D3" t="n">
-        <v>2.4635</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.4905</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="D3">
+        <v>2.4634999999999998</v>
+      </c>
+      <c r="E3">
+        <v>2.4904999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>-0.4579</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>-0.45789999999999997</v>
+      </c>
+      <c r="D4">
         <v>-0.2107</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.7895</v>
+      <c r="E4">
+        <v>-0.78949999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the computer lab x and y values
</commit_message>
<xml_diff>
--- a/output/output_parametric_survival_model_parameters.xlsx
+++ b/output/output_parametric_survival_model_parameters.xlsx
@@ -1,72 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/ahem_r_assignments/output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33186EEE-5D74-0943-AC95-B49037FC63A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="660" windowWidth="13120" windowHeight="7040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="PFS caba" sheetId="1" r:id="rId1"/>
-    <sheet name="PFS mito" sheetId="2" r:id="rId2"/>
-    <sheet name="OS caba" sheetId="3" r:id="rId3"/>
-    <sheet name="OS mito" sheetId="4" r:id="rId4"/>
+    <sheet name="PFS caba" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PFS mito" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="OS caba" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="OS mito" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>exponential</t>
-  </si>
-  <si>
-    <t>weibull</t>
-  </si>
-  <si>
-    <t>lognormal</t>
-  </si>
-  <si>
-    <t>loglogistic</t>
-  </si>
-  <si>
-    <t>AIC</t>
-  </si>
-  <si>
-    <t>intercept</t>
-  </si>
-  <si>
-    <t>log(scale)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">exponential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weibull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loglogistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log(scale)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -102,15 +82,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -392,19 +363,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FFFF7F50"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,74 +390,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1885.1070999999999</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="n">
+        <v>1885.1071</v>
+      </c>
+      <c r="C2" t="n">
         <v>1885.5943</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1886.6016</v>
       </c>
-      <c r="E2">
-        <v>1895.3381999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="n">
+        <v>1895.3382</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1.4560999999999999</v>
-      </c>
-      <c r="C3">
-        <v>1.4382999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.92820000000000003</v>
-      </c>
-      <c r="E3">
-        <v>0.93820000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="n">
+        <v>1.4561</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.4383</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9282</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9382</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>5.6599999999999998E-2</v>
-      </c>
-      <c r="D4">
+      <c r="B4"/>
+      <c r="C4" t="n">
+        <v>0.0566</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.1527</v>
       </c>
-      <c r="E4">
-        <v>-0.34789999999999999</v>
+      <c r="E4" t="n">
+        <v>-0.3479</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FFCD5B45"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,74 +473,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1754.2742000000001</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="n">
+        <v>1754.2742</v>
+      </c>
+      <c r="C2" t="n">
         <v>1748.7375</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1691.7935</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>1695.7627</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>1.1368</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>1.0851</v>
       </c>
-      <c r="D3">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="n">
+        <v>0.584</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.5222</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="B4"/>
+      <c r="C4" t="n">
         <v>0.1132</v>
       </c>
-      <c r="D4">
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="E4">
+      <c r="D4" t="n">
+        <v>0.0635</v>
+      </c>
+      <c r="E4" t="n">
         <v>-0.4662</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FF87CEEB"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,74 +556,73 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1987.5033000000001</v>
-      </c>
-      <c r="C2">
-        <v>1939.5374999999999</v>
-      </c>
-      <c r="D2">
+      <c r="B2" t="n">
+        <v>1987.5033</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1939.5375</v>
+      </c>
+      <c r="D2" t="n">
         <v>1952.9809</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>1938.9274</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>3.0550999999999999</v>
-      </c>
-      <c r="C3">
-        <v>3.0125000000000002</v>
-      </c>
-      <c r="D3">
-        <v>2.7050000000000001</v>
-      </c>
-      <c r="E3">
-        <v>2.7229999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="n">
+        <v>3.0551</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.0125</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.705</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.723</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>-0.40500000000000003</v>
-      </c>
-      <c r="D4">
+      <c r="B4"/>
+      <c r="C4" t="n">
+        <v>-0.405</v>
+      </c>
+      <c r="D4" t="n">
         <v>-0.1</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>-0.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FF4A708B"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,56 +639,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>2019.9897000000001</v>
-      </c>
-      <c r="C2">
-        <v>1948.8255999999999</v>
-      </c>
-      <c r="D2">
-        <v>1966.3670999999999</v>
-      </c>
-      <c r="E2">
+      <c r="B2" t="n">
+        <v>2019.9897</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1948.8256</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1966.3671</v>
+      </c>
+      <c r="E2" t="n">
         <v>1948.9386</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2.7684000000000002</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="n">
+        <v>2.7684</v>
+      </c>
+      <c r="C3" t="n">
         <v>2.778</v>
       </c>
-      <c r="D3">
-        <v>2.4634999999999998</v>
-      </c>
-      <c r="E3">
-        <v>2.4904999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" t="n">
+        <v>2.4635</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.4905</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>-0.45789999999999997</v>
-      </c>
-      <c r="D4">
+      <c r="B4"/>
+      <c r="C4" t="n">
+        <v>-0.4579</v>
+      </c>
+      <c r="D4" t="n">
         <v>-0.2107</v>
       </c>
-      <c r="E4">
-        <v>-0.78949999999999998</v>
+      <c r="E4" t="n">
+        <v>-0.7895</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improve code & solutions
</commit_message>
<xml_diff>
--- a/output/output_parametric_survival_model_parameters.xlsx
+++ b/output/output_parametric_survival_model_parameters.xlsx
@@ -1,52 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/ahem_r_assignments/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74637166-DBFF-5040-B117-6E01C5453D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1100" yWindow="660" windowWidth="13120" windowHeight="6100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PFS_caba" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PFS_mito" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="OS_caba" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="OS_mito" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PFS_caba" sheetId="1" r:id="rId1"/>
+    <sheet name="PFS_mito" sheetId="2" r:id="rId2"/>
+    <sheet name="OS_caba" sheetId="3" r:id="rId3"/>
+    <sheet name="OS_mito" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
-    <t xml:space="preserve"/>
+    <t/>
   </si>
   <si>
-    <t xml:space="preserve">exponential</t>
+    <t>exponential</t>
   </si>
   <si>
-    <t xml:space="preserve">weibull</t>
+    <t>weibull</t>
   </si>
   <si>
-    <t xml:space="preserve">lognormal</t>
+    <t>lognormal</t>
   </si>
   <si>
-    <t xml:space="preserve">loglogistic</t>
+    <t>loglogistic</t>
   </si>
   <si>
-    <t xml:space="preserve">AIC</t>
+    <t>AIC</t>
   </si>
   <si>
-    <t xml:space="preserve">intercept</t>
+    <t>intercept</t>
   </si>
   <si>
-    <t xml:space="preserve">log(scale)</t>
+    <t>log(scale)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -82,6 +89,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -363,17 +379,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF7F50"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,73 +408,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1885.1071</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1885.1070999999999</v>
+      </c>
+      <c r="C2">
         <v>1885.5943</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1886.6016</v>
       </c>
-      <c r="E2" t="n">
-        <v>1895.3382</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="E2">
+        <v>1895.3381999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.4561</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.4383</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.9282</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.9382</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>1.4560999999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.4382999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.92820000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0.93820000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>0.0566</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="D4">
         <v>0.1527</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.3479</v>
+      <c r="E4">
+        <v>-0.34789999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFCD5B45"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,73 +492,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1754.2742</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1754.2742000000001</v>
+      </c>
+      <c r="C2">
         <v>1748.7375</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1691.7935</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1695.7627</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1.1368</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>1.0851</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.584</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E3">
         <v>0.5222</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.1132</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.0635</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="E4">
         <v>-0.4662</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF87CEEB"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,73 +576,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>1987.5033</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1939.5375</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B2">
+        <v>1987.5033000000001</v>
+      </c>
+      <c r="C2">
+        <v>1939.5374999999999</v>
+      </c>
+      <c r="D2">
         <v>1952.9809</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1938.9274</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>3.0551</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3.0125</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.705</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.723</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>3.0550999999999999</v>
+      </c>
+      <c r="C3">
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="D3">
+        <v>2.7050000000000001</v>
+      </c>
+      <c r="E3">
+        <v>2.7229999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>-0.405</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>-0.40500000000000003</v>
+      </c>
+      <c r="D4">
         <v>-0.1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>-0.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF4A708B"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,57 +660,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
-        <v>2019.9897</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1948.8256</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1966.3671</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="B2">
+        <v>2019.9897000000001</v>
+      </c>
+      <c r="C2">
+        <v>1948.8255999999999</v>
+      </c>
+      <c r="D2">
+        <v>1966.3670999999999</v>
+      </c>
+      <c r="E2">
         <v>1948.9386</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
-        <v>2.7684</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3">
+        <v>2.7684000000000002</v>
+      </c>
+      <c r="C3">
         <v>2.778</v>
       </c>
-      <c r="D3" t="n">
-        <v>2.4635</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.4905</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="D3">
+        <v>2.4634999999999998</v>
+      </c>
+      <c r="E3">
+        <v>2.4904999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="n">
-        <v>-0.4579</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>-0.45789999999999997</v>
+      </c>
+      <c r="D4">
         <v>-0.2107</v>
       </c>
-      <c r="E4" t="n">
-        <v>-0.7895</v>
+      <c r="E4">
+        <v>-0.78949999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>